<commit_message>
decorated excle file approriate properties
</commit_message>
<xml_diff>
--- a/keywords.xlsx
+++ b/keywords.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="GmailKeywords" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,10 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>Keywords</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>Description</t>
   </si>
@@ -49,6 +46,42 @@
   </si>
   <si>
     <t>Compose email message</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Keyword</t>
+  </si>
+  <si>
+    <t>Operation</t>
+  </si>
+  <si>
+    <t>Set value</t>
+  </si>
+  <si>
+    <t>Click</t>
+  </si>
+  <si>
+    <t>Function</t>
+  </si>
+  <si>
+    <t>Run app</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>TestCase Name</t>
+  </si>
+  <si>
+    <t>TC_01</t>
+  </si>
+  <si>
+    <t>Data Set</t>
   </si>
 </sst>
 </file>
@@ -84,8 +117,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -366,56 +405,119 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.42578125" customWidth="1"/>
-    <col min="2" max="2" width="24.140625" customWidth="1"/>
+    <col min="2" max="2" width="7" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+    <col min="5" max="5" width="27.140625" customWidth="1"/>
+    <col min="6" max="6" width="31.7109375" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="H1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="1">
         <v>1</v>
       </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2">
         <v>3</v>
       </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="D6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
was added additional methods
</commit_message>
<xml_diff>
--- a/keywords.xlsx
+++ b/keywords.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="22">
   <si>
     <t>Description</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>Data Set</t>
+  </si>
+  <si>
+    <t>TC_02</t>
   </si>
 </sst>
 </file>
@@ -405,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -520,6 +523,78 @@
         <v>8</v>
       </c>
     </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2">
+        <v>3</v>
+      </c>
+      <c r="D9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="D11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
was made some excle unmarshallong arhitecture
</commit_message>
<xml_diff>
--- a/keywords.xlsx
+++ b/keywords.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>Description</t>
   </si>
@@ -30,9 +30,6 @@
     <t>Login to gmail site</t>
   </si>
   <si>
-    <t>Emails</t>
-  </si>
-  <si>
     <t>Delete</t>
   </si>
   <si>
@@ -82,9 +79,6 @@
   </si>
   <si>
     <t>Data Set</t>
-  </si>
-  <si>
-    <t>TC_02</t>
   </si>
 </sst>
 </file>
@@ -411,7 +405,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -427,42 +421,42 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" t="s">
-        <v>12</v>
-      </c>
       <c r="F1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G1" t="s">
         <v>0</v>
       </c>
       <c r="H1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
         <v>15</v>
-      </c>
-      <c r="D2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -474,7 +468,7 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G3" t="s">
         <v>2</v>
@@ -486,13 +480,13 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -501,101 +495,47 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
-      <c r="D6" t="s">
-        <v>6</v>
-      </c>
       <c r="E6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="1">
-        <v>1</v>
-      </c>
-      <c r="C7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" t="s">
-        <v>16</v>
-      </c>
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
-      <c r="B8" s="2">
-        <v>2</v>
-      </c>
-      <c r="D8" t="s">
-        <v>1</v>
-      </c>
-      <c r="E8" t="s">
-        <v>13</v>
-      </c>
-      <c r="G8" t="s">
-        <v>2</v>
-      </c>
+      <c r="B8" s="2"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
-      <c r="B9" s="2">
-        <v>3</v>
-      </c>
-      <c r="D9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G9" t="s">
-        <v>5</v>
-      </c>
+      <c r="B9" s="2"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
-      <c r="B10" s="2">
-        <v>4</v>
-      </c>
-      <c r="D10" t="s">
-        <v>4</v>
-      </c>
-      <c r="E10" t="s">
-        <v>14</v>
-      </c>
-      <c r="G10" t="s">
-        <v>7</v>
-      </c>
+      <c r="B10" s="2"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
-      <c r="D11" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11" t="s">
-        <v>14</v>
-      </c>
-      <c r="G11" t="s">
-        <v>8</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>